<commit_message>
Completed Tumble Buggy assignment
</commit_message>
<xml_diff>
--- a/6-Honors_Physics/tumble_buggy_position_vs_time/tumble_buggy_position_vs_time.xlsx
+++ b/6-Honors_Physics/tumble_buggy_position_vs_time/tumble_buggy_position_vs_time.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ladmin/courses/6-Honors_Physics/kinematics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ladmin/courses/6-Honors_Physics/tumble_buggy_position_vs_time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A123659-B57B-6843-AE4A-E038AA7CDEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8F8891-9422-6649-8EA4-EB7E9ED9CA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" xr2:uid="{CE019F0A-D800-ED46-9B74-27FF723504C5}"/>
   </bookViews>
@@ -69,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,12 +77,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,10 +251,43 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.17127475708990414"/>
-                  <c:y val="-9.3009259259259264E-2"/>
+                  <c:x val="0.16273704296712216"/>
+                  <c:y val="-0.1300462962962963"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x = 0.2941(m/s)t</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>R² = 0.9977</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:solidFill>
@@ -379,10 +430,43 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.16848924176956989"/>
-                  <c:y val="1.6254738990959465E-2"/>
+                  <c:x val="0.172806571184173"/>
+                  <c:y val="0.17366214639836688"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x= 0.2741(m/s)t</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>R² = 0.9956</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:solidFill>
@@ -523,10 +607,43 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.16552255828745652"/>
-                  <c:y val="9.9620516185476862E-2"/>
+                  <c:x val="0.16855876998662075"/>
+                  <c:y val="0.26165755322251383"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x = 0.245(m/s)t</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>R² = 0.9971</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:solidFill>
@@ -784,20 +901,29 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>Position</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> (m)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -821,9 +947,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1521,7 +1647,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>490220</xdr:colOff>
+      <xdr:colOff>802640</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>149860</xdr:rowOff>
     </xdr:to>
@@ -1851,92 +1977,92 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.71</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.75700000000000001</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1.27</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1.25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1.01</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1.85</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.62</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1.54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2.35</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>2.17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1.98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2.83</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2.67</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>2.35</v>
       </c>
     </row>

</xml_diff>